<commit_message>
Završena stranica za izvode
</commit_message>
<xml_diff>
--- a/ProgramZaRacunovodstvo/Template/Template.xlsx
+++ b/ProgramZaRacunovodstvo/Template/Template.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Redni br.</t>
   </si>
   <si>
-    <t>Naziv fakture</t>
-  </si>
-  <si>
     <t>Pravno lice</t>
   </si>
   <si>
@@ -37,32 +34,44 @@
     <t>Datum slanja</t>
   </si>
   <si>
-    <t>Ulazni PDV:</t>
-  </si>
-  <si>
-    <t>Ulazne fakture:</t>
-  </si>
-  <si>
-    <t>Izlazne fakture</t>
-  </si>
-  <si>
-    <t>Izlazni PDV:</t>
-  </si>
-  <si>
-    <t>Ukupno:</t>
-  </si>
-  <si>
     <t>Tip fakture</t>
   </si>
   <si>
     <t>Izvod: 25.02.2025-03.03.2025.</t>
+  </si>
+  <si>
+    <t>Broj fakture</t>
+  </si>
+  <si>
+    <t>Prodaja bez PDV-a:</t>
+  </si>
+  <si>
+    <t>Prodaja PDV:</t>
+  </si>
+  <si>
+    <t>Prodaja ukupno:</t>
+  </si>
+  <si>
+    <t>Nabavke bez PDV-a:</t>
+  </si>
+  <si>
+    <t>Nabavke PDV:</t>
+  </si>
+  <si>
+    <t>Nabavke ukupno:</t>
+  </si>
+  <si>
+    <t>Stanje PDV:</t>
+  </si>
+  <si>
+    <t>Promet:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +82,14 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -94,7 +111,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -227,144 +244,23 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -391,6 +287,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,137 +630,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J15"/>
+  <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H24" sqref="H24:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
     <col min="10" max="10" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="36.75" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:10" ht="15.75" thickTop="1">
-      <c r="B2" s="14" t="s">
+    <row r="1" spans="2:11" ht="36.75" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:11" ht="15.75" thickTop="1">
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="2:11" ht="30.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:11" ht="21.75" customHeight="1" thickTop="1">
+      <c r="B7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="2:11" ht="15.75" thickTop="1">
+      <c r="B9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="2:11" ht="21.75" customHeight="1" thickBot="1">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" thickTop="1">
+      <c r="B11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="2:11" ht="21.75" customHeight="1" thickBot="1">
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="2:11" ht="16.5" thickTop="1" thickBot="1">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="2:11" ht="21.75" customHeight="1" thickTop="1">
+      <c r="B14" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="25"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B15" s="24"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="26"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="2:11" ht="15.75" thickTop="1">
+      <c r="B16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="2:10">
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-    </row>
-    <row r="5" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" thickTop="1">
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="8" spans="2:10" ht="15.75" thickTop="1">
-      <c r="I8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" thickBot="1">
-      <c r="I9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" thickTop="1">
-      <c r="I11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="2:10" ht="15.75" thickBot="1">
-      <c r="I12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="I14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="2:10" ht="15.75" thickTop="1"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="25"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="2:9" ht="21.75" customHeight="1" thickBot="1">
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" thickTop="1">
+      <c r="B18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="2:9" ht="21.75" customHeight="1" thickBot="1">
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="26"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1"/>
+    <row r="21" spans="2:9" ht="21.75" customHeight="1" thickTop="1">
+      <c r="B21" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="25"/>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="2:9" ht="16.5" thickTop="1" thickBot="1"/>
+    <row r="24" spans="2:9" ht="21.75" customHeight="1" thickTop="1">
+      <c r="B24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="28"/>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="30"/>
+    </row>
+    <row r="26" spans="2:9" ht="15.75" thickTop="1"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="17">
+    <mergeCell ref="B24:G25"/>
+    <mergeCell ref="H24:I25"/>
+    <mergeCell ref="B18:G19"/>
+    <mergeCell ref="H18:I19"/>
+    <mergeCell ref="B21:G22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="B11:G12"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="B14:G15"/>
+    <mergeCell ref="H14:I15"/>
+    <mergeCell ref="B16:G17"/>
+    <mergeCell ref="H16:I17"/>
     <mergeCell ref="B2:I4"/>
+    <mergeCell ref="B7:G8"/>
+    <mergeCell ref="H7:I8"/>
+    <mergeCell ref="B9:G10"/>
+    <mergeCell ref="H9:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>